<commit_message>
Code for Temperature Plot
It contains the code for plotting temperature data.
</commit_message>
<xml_diff>
--- a/Dataset/temperature_data.xlsx
+++ b/Dataset/temperature_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github Folder\githubtestsulove\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{710B8AA1-CA8D-48F0-B221-12326BF5D8A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83AE0B24-138C-4768-B37D-69C6959F0A04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28692" yWindow="-108" windowWidth="25416" windowHeight="15972" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,13 +41,13 @@
     <t>Group</t>
   </si>
   <si>
-    <t>A</t>
+    <t>Animal_ID</t>
   </si>
   <si>
-    <t>B</t>
+    <t>Group A</t>
   </si>
   <si>
-    <t>Animal_ID</t>
+    <t>Group B</t>
   </si>
 </sst>
 </file>
@@ -381,7 +381,7 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="C2:K15"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -391,7 +391,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -429,7 +429,7 @@
         <v>97</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="2">
         <v>39.5</v>
@@ -464,7 +464,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" s="2">
         <v>39.700000000000003</v>
@@ -499,7 +499,7 @@
         <v>94</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" s="2">
         <v>37.200000000000003</v>
@@ -534,7 +534,7 @@
         <v>66</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" s="2">
         <v>39.299999999999997</v>
@@ -566,10 +566,10 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" s="2">
         <v>37.4</v>
@@ -604,7 +604,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" s="2">
         <v>38.200000000000003</v>
@@ -639,7 +639,7 @@
         <v>76</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" s="2">
         <v>39.200000000000003</v>
@@ -674,13 +674,13 @@
         <v>84</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C9" s="2">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D9" s="2">
-        <v>42.1</v>
+        <v>40</v>
       </c>
       <c r="E9" s="2">
         <v>41.5</v>
@@ -709,13 +709,13 @@
         <v>61</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C10" s="2">
-        <v>40.799999999999997</v>
+        <v>37.1</v>
       </c>
       <c r="D10" s="2">
-        <v>39.299999999999997</v>
+        <v>39.700000000000003</v>
       </c>
       <c r="E10" s="2">
         <v>39.1</v>
@@ -744,13 +744,13 @@
         <v>99</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C11" s="2">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D11" s="2">
-        <v>41.6</v>
+        <v>39.5</v>
       </c>
       <c r="E11" s="2">
         <v>41.4</v>
@@ -779,13 +779,13 @@
         <v>39</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C12" s="2">
-        <v>40.4</v>
+        <v>38.5</v>
       </c>
       <c r="D12" s="2">
-        <v>39.1</v>
+        <v>39.5</v>
       </c>
       <c r="E12" s="2">
         <v>40.5</v>
@@ -811,16 +811,16 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C13" s="2">
-        <v>39.5</v>
+        <v>37.799999999999997</v>
       </c>
       <c r="D13" s="2">
-        <v>41.6</v>
+        <v>38</v>
       </c>
       <c r="E13" s="2">
         <v>41</v>
@@ -849,13 +849,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C14" s="2">
-        <v>40.799999999999997</v>
+        <v>39</v>
       </c>
       <c r="D14" s="2">
-        <v>41.7</v>
+        <v>39.700000000000003</v>
       </c>
       <c r="E14" s="2">
         <v>41.5</v>
@@ -884,10 +884,10 @@
         <v>7</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C15" s="2">
-        <v>42.6</v>
+        <v>38.799999999999997</v>
       </c>
       <c r="D15" s="2">
         <v>39.799999999999997</v>

</xml_diff>